<commit_message>
excel generator finished, maybe needs more fields, is returning the file name
</commit_message>
<xml_diff>
--- a/reports/report_template.xlsx
+++ b/reports/report_template.xlsx
@@ -24,19 +24,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MRN</t>
   </si>
   <si>
     <t>Appt</t>
+  </si>
+  <si>
+    <t>WR Time</t>
+  </si>
+  <si>
+    <t>EX Time</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Needs Imaging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,28 +56,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -73,30 +73,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,20 +359,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added imaging fields to the report
</commit_message>
<xml_diff>
--- a/reports/report_template.xlsx
+++ b/reports/report_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>MRN</t>
   </si>
@@ -33,31 +33,37 @@
     <t xml:space="preserve"> Appt Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> WR timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EX timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FC Timestamp start</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FC Timestamp end</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DC Timestamp</t>
   </si>
   <si>
-    <t xml:space="preserve"> WR total time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EX total time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FC total time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AT entry</t>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EX Total Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WR Total Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WR Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EX Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AT Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FC Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FC End</t>
+  </si>
+  <si>
+    <t>Imaging</t>
+  </si>
+  <si>
+    <t>Imaging Timestamp</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -375,16 +381,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,31 +415,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding imaging start field in the excel report
</commit_message>
<xml_diff>
--- a/reports/report_template.xlsx
+++ b/reports/report_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Buailteoir\Documents\Imbas\Orthopaedics\orthopaedics\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>MRN</t>
   </si>
@@ -64,12 +69,15 @@
   </si>
   <si>
     <t>Imaging Timestamp</t>
+  </si>
+  <si>
+    <t>Imaging Start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,12 +404,13 @@
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,18 +442,21 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added momentJS to excelController. Filtering patients with apptLoc=EXP. Added fields to patient report. Changed labels on patient report.
</commit_message>
<xml_diff>
--- a/reports/report_template.xlsx
+++ b/reports/report_template.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Buailteoir\Documents\Imbas\Orthopaedics\orthopaedics\reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34980" windowHeight="13280"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PatientStats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,38 +22,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>MRN</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nombre</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Physician</t>
   </si>
   <si>
     <t xml:space="preserve"> Appt Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> DC Timestamp</t>
-  </si>
-  <si>
     <t>Total Time</t>
   </si>
   <si>
     <t xml:space="preserve"> EX Total Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> WR Total Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WR Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EX Timestamp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> AT Entry</t>
   </si>
   <si>
@@ -65,23 +48,57 @@
     <t xml:space="preserve"> FC End</t>
   </si>
   <si>
-    <t>Imaging</t>
-  </si>
-  <si>
-    <t>Imaging Timestamp</t>
-  </si>
-  <si>
-    <t>Imaging Start</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Imaging Start Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Register Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Call Back Timestamp</t>
+  </si>
+  <si>
+    <t>Discharge Timestamp</t>
+  </si>
+  <si>
+    <t>Imaging End Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Appt Type</t>
+  </si>
+  <si>
+    <t>Imaging Total Time</t>
+  </si>
+  <si>
+    <t>Callback vs. Appt Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,13 +121,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -389,45 +426,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
@@ -436,31 +475,40 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
         <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
separates date and time from appt time
</commit_message>
<xml_diff>
--- a/reports/report_template.xlsx
+++ b/reports/report_template.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Buailteoir\Documents\Imbas\Orthopaedics\orthopaedics\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34980" windowHeight="13280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34980" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="PatientStats" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>MRN</t>
   </si>
@@ -76,12 +81,15 @@
   </si>
   <si>
     <t>Physician Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Appt Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -433,31 +441,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,45 +479,48 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>